<commit_message>
included pagination and code optimization
</commit_message>
<xml_diff>
--- a/src/test/resources/excelReader/Elimination&AddList.xlsx
+++ b/src/test/resources/excelReader/Elimination&AddList.xlsx
@@ -4,6 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Diabetes Elimination" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Hypothyroidism Elimination" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Hypertension Elimination" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="PCOS Elimination" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
   <si>
     <t>Processed grains - cream of rice, rice flour, rice rava, corn</t>
   </si>
@@ -107,6 +110,147 @@
   </si>
   <si>
     <t>Dairy Milk, butter, cheese</t>
+  </si>
+  <si>
+    <t>Tofu</t>
+  </si>
+  <si>
+    <t>Edamame</t>
+  </si>
+  <si>
+    <t>Tempeh</t>
+  </si>
+  <si>
+    <t>Cauliflower</t>
+  </si>
+  <si>
+    <t>Cabbage</t>
+  </si>
+  <si>
+    <t>Broccoli</t>
+  </si>
+  <si>
+    <t>Kale</t>
+  </si>
+  <si>
+    <t>Spinach</t>
+  </si>
+  <si>
+    <t>Sweet potatoes</t>
+  </si>
+  <si>
+    <t>Strawberries</t>
+  </si>
+  <si>
+    <t>Pine nuts</t>
+  </si>
+  <si>
+    <t>Peanuts</t>
+  </si>
+  <si>
+    <t>Peaches</t>
+  </si>
+  <si>
+    <t>Green tea</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Alcohol</t>
+  </si>
+  <si>
+    <t>Soy milk</t>
+  </si>
+  <si>
+    <t>Cakes, pastries</t>
+  </si>
+  <si>
+    <t>Fried food</t>
+  </si>
+  <si>
+    <t>Processed food- ham, bacon, salami, sausages</t>
+  </si>
+  <si>
+    <t>Frozen food</t>
+  </si>
+  <si>
+    <t>Gluten</t>
+  </si>
+  <si>
+    <t>Sodas</t>
+  </si>
+  <si>
+    <t>Energy drinks containing caffeine</t>
+  </si>
+  <si>
+    <t>Packaged food- noodles, soups, salad dressings, sauces</t>
+  </si>
+  <si>
+    <t>Salty food/snacks(chips,pretzels,crackers)</t>
+  </si>
+  <si>
+    <t>Caffeine-coffee/tea &amp; many soft drinks</t>
+  </si>
+  <si>
+    <t>Frozen food, meat (bacon, ham)</t>
+  </si>
+  <si>
+    <t>Pickles</t>
+  </si>
+  <si>
+    <t>Processed/canned food</t>
+  </si>
+  <si>
+    <t>Sauces, mayonnaise</t>
+  </si>
+  <si>
+    <t>Processed meat(bacon,sausages,deli meats)</t>
+  </si>
+  <si>
+    <t>White rice,</t>
+  </si>
+  <si>
+    <t>white bread</t>
+  </si>
+  <si>
+    <t>Cakes</t>
+  </si>
+  <si>
+    <t>Pastries</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Burger</t>
+  </si>
+  <si>
+    <t>Carbonated beverages</t>
+  </si>
+  <si>
+    <t>Sugary foods (sweets, icecreams) and beverages (soda, juices)</t>
+  </si>
+  <si>
+    <t>Red meat</t>
+  </si>
+  <si>
+    <t>Processed meat</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>Soy products</t>
+  </si>
+  <si>
+    <t>Doughnuts</t>
+  </si>
+  <si>
+    <t>Fries</t>
+  </si>
+  <si>
+    <t>Seed oils- vegetable oil, soybean oil, canola oil, rapeseed oil, sunflower oil, safflower oil</t>
   </si>
 </sst>
 </file>
@@ -139,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border/>
     <border>
       <left style="thin">
@@ -166,11 +310,22 @@
         <color rgb="FFAAAAAA"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -183,6 +338,9 @@
     <xf borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -192,6 +350,18 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -565,4 +735,339 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>